<commit_message>
remove ngayhh trong giay_dc_diaphuong
</commit_message>
<xml_diff>
--- a/public/FileImportMilitary/DC_DiaPhuong.xlsx
+++ b/public/FileImportMilitary/DC_DiaPhuong.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Tai lieu\NCKH_K60\TaiLieuTestCode\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Tai lieu\NCKH_K60\File_Code\NCKH\Backend_NCKH\public\FileImportMilitary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F4D72B6-9746-47EB-89DB-0D2ABE61ABF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D6939A-4637-462E-B82A-5721F4C7BEA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E432A2BE-2905-466D-81D6-202721194E44}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
   <si>
     <t>stt</t>
   </si>
@@ -45,9 +45,6 @@
     <t>ngày cấp</t>
   </si>
   <si>
-    <t>ngày hết hạn</t>
-  </si>
-  <si>
     <t>nơi ở hiện tại</t>
   </si>
   <si>
@@ -63,16 +60,67 @@
     <t>mã giấy đăng ký</t>
   </si>
   <si>
-    <t>Cầu giấy hà nội</t>
-  </si>
-  <si>
-    <t>Ban CHQS phường quan hoa</t>
-  </si>
-  <si>
     <t>Trúng tuyển đại học cao đẳng</t>
   </si>
   <si>
-    <t>Trường DH GTVT</t>
+    <t>Vạn Điểm, Thường tín, Hà Nội</t>
+  </si>
+  <si>
+    <t>Trường ĐH GTVT</t>
+  </si>
+  <si>
+    <t>Khu Quán Gỏi, xã Hưng Thịnh, Bình Giang, Hải Dương</t>
+  </si>
+  <si>
+    <t>BCHQS XÃ HƯNG THỊNH</t>
+  </si>
+  <si>
+    <t>BCHQS XÃ VẠN ĐIỂM</t>
+  </si>
+  <si>
+    <t>Ấp Đông Côi, Thị trấn Hồ, Thuận Thành, Bắc Ninh</t>
+  </si>
+  <si>
+    <t>Ban CHQS THỊ TRẤN HỒ</t>
+  </si>
+  <si>
+    <t>Thôn 1, Đông Mỹ, Thanh Trì, Hà Nội</t>
+  </si>
+  <si>
+    <t>BAN CHQS XÃ ĐÔNG MỸ</t>
+  </si>
+  <si>
+    <t>Lạc Thổ Nam, Thị trấn Hồ, Thuận Thành, Bắc Ninh</t>
+  </si>
+  <si>
+    <t>số 9 ngách 99/3 Nguyễn Chí Thanh, Láng Hạ, Đống Đa, Hà Nội</t>
+  </si>
+  <si>
+    <t>BAN CHQS PHƯỜNG LÁNG HẠ</t>
+  </si>
+  <si>
+    <t>Vũ Hòa, Kiến Xương, Thái Bình</t>
+  </si>
+  <si>
+    <t>BAN CHQS XÃ VŨ HÒA</t>
+  </si>
+  <si>
+    <t>Thôn Thống Nhất, Thành Vinh, Thạch Thành, Thanh Hóa</t>
+  </si>
+  <si>
+    <t>BAN CHQS XÃ THÀNH VINH</t>
+  </si>
+  <si>
+    <t>thôn Thống nhất, xã Phương Khoan, huyện Sông Lô, Vĩnh Phúc</t>
+  </si>
+  <si>
+    <t>BAN CHQS XÃ PHƯƠNG KHOAN</t>
+  </si>
+  <si>
+    <t>BAN CHQS XÃ MINH THANH</t>
+  </si>
+  <si>
+    <t>thôn Lê, xã Minh Thanh, Sơn Dương, Tuyên Quang</t>
   </si>
 </sst>
 </file>
@@ -425,25 +473,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09C63CFA-5EB6-4135-9FE7-621954B2F8AB}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:H71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="13.33203125" customWidth="1"/>
     <col min="3" max="3" width="15.9140625" customWidth="1"/>
-    <col min="4" max="4" width="17.25" customWidth="1"/>
-    <col min="5" max="5" width="17.5" customWidth="1"/>
-    <col min="6" max="6" width="17.1640625" customWidth="1"/>
-    <col min="7" max="7" width="26.83203125" customWidth="1"/>
-    <col min="8" max="8" width="24.5" customWidth="1"/>
-    <col min="9" max="9" width="17.4140625" customWidth="1"/>
+    <col min="4" max="4" width="52.75" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" customWidth="1"/>
+    <col min="6" max="6" width="26.83203125" customWidth="1"/>
+    <col min="7" max="7" width="28.83203125" customWidth="1"/>
+    <col min="8" max="8" width="17.4140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -468,37 +515,745 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>88</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>44125</v>
-      </c>
-      <c r="D2" s="1">
-        <v>44186</v>
+        <v>43696</v>
+      </c>
+      <c r="D2" t="s">
+        <v>28</v>
       </c>
       <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1">
+        <v>44148</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>43691</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1">
+        <v>43693</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>24</v>
+      </c>
+      <c r="C6" s="1">
+        <v>43692</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>15</v>
+      </c>
+      <c r="C7" s="1">
+        <v>43691</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1">
+        <v>43689</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1">
+        <v>43690</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" s="1">
+        <v>43689</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>17</v>
+      </c>
+      <c r="C11" s="1">
+        <v>43693</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12">
         <v>11</v>
       </c>
-      <c r="H2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2">
-        <v>3</v>
+      <c r="H12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="H13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="H14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="H15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="H16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="H17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="H18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="H19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="H20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="H21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="H22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="H23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="H24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="H25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="H26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="H27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="H28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="H29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="H30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="H31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="H32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="H33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="H34">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="H35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="H36">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="H37">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="H38">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="H39">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="H40">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="H41">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="H42">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="H43">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="H44">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="H45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="H46">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="H47">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="H48">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="H49">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="H50">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="H51">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="H52">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="H53">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="H54">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="H55">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="H56">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="H57">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="H58">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="H59">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="H60">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="H61">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="H62">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="H63">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="H64">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="H65">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="H66">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="H67">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="H68">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="H69">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="H70">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="H71">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>